<commit_message>
Updated faculty data for 3-2 semester with real faculty list
</commit_message>
<xml_diff>
--- a/server/attendance_sheets/FAC001_3_2_Data_Structures.xlsx
+++ b/server/attendance_sheets/FAC001_3_2_Data_Structures.xlsx
@@ -832,7 +832,7 @@
         <v>A</v>
       </c>
       <c r="M2" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="N2" t="str">
         <v/>
@@ -1177,10 +1177,10 @@
         <v>8</v>
       </c>
       <c r="DX2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DY2" t="str">
-        <v>88.9%</v>
+        <v>80.0%</v>
       </c>
     </row>
     <row r="3">
@@ -1197,7 +1197,7 @@
         <v>P</v>
       </c>
       <c r="E3" t="str">
-        <v>P</v>
+        <v>A</v>
       </c>
       <c r="F3" t="str">
         <v>P</v>
@@ -1221,7 +1221,7 @@
         <v>A</v>
       </c>
       <c r="M3" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="N3" t="str">
         <v/>
@@ -1566,10 +1566,10 @@
         <v>8</v>
       </c>
       <c r="DX3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DY3" t="str">
-        <v>88.9%</v>
+        <v>80.0%</v>
       </c>
     </row>
     <row r="4">
@@ -1586,7 +1586,7 @@
         <v>P</v>
       </c>
       <c r="E4" t="str">
-        <v>P</v>
+        <v>A</v>
       </c>
       <c r="F4" t="str">
         <v>P</v>
@@ -1610,7 +1610,7 @@
         <v>A</v>
       </c>
       <c r="M4" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="N4" t="str">
         <v/>
@@ -1955,10 +1955,10 @@
         <v>8</v>
       </c>
       <c r="DX4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DY4" t="str">
-        <v>88.9%</v>
+        <v>80.0%</v>
       </c>
     </row>
     <row r="5">
@@ -1999,7 +1999,7 @@
         <v>A</v>
       </c>
       <c r="M5" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="N5" t="str">
         <v/>
@@ -2344,10 +2344,10 @@
         <v>8</v>
       </c>
       <c r="DX5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DY5" t="str">
-        <v>88.9%</v>
+        <v>80.0%</v>
       </c>
     </row>
     <row r="6">
@@ -2388,7 +2388,7 @@
         <v>A</v>
       </c>
       <c r="M6" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="N6" t="str">
         <v/>
@@ -2733,10 +2733,10 @@
         <v>8</v>
       </c>
       <c r="DX6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DY6" t="str">
-        <v>88.9%</v>
+        <v>80.0%</v>
       </c>
     </row>
     <row r="7">
@@ -2777,7 +2777,7 @@
         <v>A</v>
       </c>
       <c r="M7" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="N7" t="str">
         <v/>
@@ -3119,13 +3119,13 @@
         <v/>
       </c>
       <c r="DW7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DX7">
         <v>1</v>
       </c>
       <c r="DY7" t="str">
-        <v>88.9%</v>
+        <v>90.0%</v>
       </c>
     </row>
     <row r="8">
@@ -3166,7 +3166,7 @@
         <v>A</v>
       </c>
       <c r="M8" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="N8" t="str">
         <v/>
@@ -3508,13 +3508,13 @@
         <v/>
       </c>
       <c r="DW8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DX8">
         <v>1</v>
       </c>
       <c r="DY8" t="str">
-        <v>88.9%</v>
+        <v>90.0%</v>
       </c>
     </row>
     <row r="9">
@@ -3555,7 +3555,7 @@
         <v>A</v>
       </c>
       <c r="M9" t="str">
-        <v/>
+        <v>A</v>
       </c>
       <c r="N9" t="str">
         <v/>
@@ -3900,10 +3900,10 @@
         <v>8</v>
       </c>
       <c r="DX9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DY9" t="str">
-        <v>88.9%</v>
+        <v>80.0%</v>
       </c>
     </row>
     <row r="10">
@@ -3944,7 +3944,7 @@
         <v>A</v>
       </c>
       <c r="M10" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="N10" t="str">
         <v/>
@@ -4286,13 +4286,13 @@
         <v/>
       </c>
       <c r="DW10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DX10">
         <v>1</v>
       </c>
       <c r="DY10" t="str">
-        <v>88.9%</v>
+        <v>90.0%</v>
       </c>
     </row>
     <row r="11">
@@ -4333,7 +4333,7 @@
         <v>A</v>
       </c>
       <c r="M11" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="N11" t="str">
         <v/>
@@ -4675,13 +4675,13 @@
         <v/>
       </c>
       <c r="DW11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="DX11">
         <v>1</v>
       </c>
       <c r="DY11" t="str">
-        <v>88.9%</v>
+        <v>90.0%</v>
       </c>
     </row>
   </sheetData>

</xml_diff>